<commit_message>
feat:up till 272 from res1 scraped
</commit_message>
<xml_diff>
--- a/scrape_urls/res1.xlsx
+++ b/scrape_urls/res1.xlsx
@@ -968,7 +968,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -991,13 +991,6 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <name val="Cambria"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1007,19 +1000,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
@@ -1053,8 +1039,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1076,1580 +1062,1578 @@
   </sheetPr>
   <dimension ref="A1:A314"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A72" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A166" activeCellId="0" sqref="A166"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A251" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H264" activeCellId="0" sqref="H264"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1"/>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="s">
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="s">
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="s">
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="s">
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0" t="s">
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="s">
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0" t="s">
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="s">
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="s">
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="s">
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="s">
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="s">
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="s">
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="s">
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0" t="s">
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="0" t="s">
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="0" t="s">
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="0" t="s">
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="0" t="s">
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="0" t="s">
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="0" t="s">
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="0" t="s">
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="0" t="s">
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="0" t="s">
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="0" t="s">
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="0" t="s">
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="0" t="s">
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="0" t="s">
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="0" t="s">
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="0" t="s">
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="0" t="s">
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="0" t="s">
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="0" t="s">
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="0" t="s">
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="0" t="s">
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="0" t="s">
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="0" t="s">
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="0" t="s">
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="0" t="s">
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="0" t="s">
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="0" t="s">
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="0" t="s">
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="0" t="s">
+    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="0" t="s">
+    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="0" t="s">
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="0" t="s">
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="0" t="s">
+    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="0" t="s">
+    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="0" t="s">
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="0" t="s">
+    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="0" t="s">
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="0" t="s">
+    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="0" t="s">
+    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="0" t="s">
+    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="0" t="s">
+    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="0" t="s">
+    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="0" t="s">
+    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="0" t="s">
+    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="0" t="s">
+    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="0" t="s">
+    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="0" t="s">
+    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="0" t="s">
+    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="0" t="s">
+    <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="0" t="s">
+    <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="0" t="s">
+    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="0" t="s">
+    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="0" t="s">
+    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="0" t="s">
+    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="0" t="s">
+    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="1" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="0" t="s">
+    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="1" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="0" t="s">
+    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A125" s="0" t="s">
+    <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="0" t="s">
+    <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="0" t="s">
+    <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="1" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A128" s="0" t="s">
+    <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="0" t="s">
+    <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="1" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="0" t="s">
+    <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="1" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="0" t="s">
+    <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="0" t="s">
+    <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="1" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="0" t="s">
+    <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="0" t="s">
+    <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="0" t="s">
+    <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="0" t="s">
+    <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A137" s="0" t="s">
+    <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="1" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="0" t="s">
+    <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="1" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="0" t="s">
+    <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="1" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A140" s="0" t="s">
+    <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="1" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A141" s="0" t="s">
+    <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="1" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A142" s="0" t="s">
+    <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="1" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="0" t="s">
+    <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="1" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="0" t="s">
+    <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="1" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="0" t="s">
+    <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="1" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A146" s="0" t="s">
+    <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="1" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A147" s="0" t="s">
+    <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A148" s="0" t="s">
+    <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A147" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A149" s="0" t="s">
+    <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A148" s="1" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A150" s="0" t="s">
+    <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="1" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A151" s="0" t="s">
+    <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A150" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A152" s="0" t="s">
+    <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A151" s="1" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A153" s="0" t="s">
+    <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A152" s="1" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A154" s="0" t="s">
+    <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A153" s="1" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A155" s="0" t="s">
+    <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="1" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A156" s="0" t="s">
+    <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="1" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A157" s="0" t="s">
+    <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="158" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A158" s="0" t="s">
+    <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A157" s="1" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="159" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A159" s="0" t="s">
+    <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="160" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A160" s="0" t="s">
+    <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A159" s="1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="161" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A161" s="0" t="s">
+    <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A160" s="1" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="162" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A162" s="0" t="s">
+    <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A161" s="1" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="163" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A163" s="0" t="s">
+    <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A162" s="1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A164" s="0" t="s">
+    <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A163" s="1" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="165" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A165" s="0" t="s">
+    <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="1" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="166" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A166" s="0" t="s">
+    <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A165" s="1" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="167" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A167" s="0" t="s">
+    <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A166" s="1" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="168" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A168" s="0" t="s">
+    <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A167" s="1" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="169" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A169" s="0" t="s">
+    <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A168" s="1" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="170" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A170" s="0" t="s">
+    <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A169" s="1" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="171" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A171" s="0" t="s">
+    <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="1" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="172" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A172" s="0" t="s">
+    <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A171" s="1" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="173" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A173" s="0" t="s">
+    <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A172" s="1" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="174" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A174" s="0" t="s">
+    <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A173" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="175" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A175" s="0" t="s">
+    <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A174" s="1" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="176" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A176" s="0" t="s">
+    <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A175" s="1" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="177" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A177" s="0" t="s">
+    <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A176" s="1" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="178" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A178" s="0" t="s">
+    <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A177" s="1" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="179" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A179" s="0" t="s">
+    <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A178" s="1" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="180" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A180" s="0" t="s">
+    <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A179" s="1" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="181" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A181" s="0" t="s">
+    <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A180" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="182" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A182" s="0" t="s">
+    <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A181" s="1" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="183" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A183" s="0" t="s">
+    <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A182" s="1" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="184" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A184" s="0" t="s">
+    <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A183" s="1" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="185" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A185" s="0" t="s">
+    <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A184" s="1" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="186" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A186" s="0" t="s">
+    <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A185" s="1" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="187" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A187" s="0" t="s">
+    <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A186" s="1" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="188" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A188" s="0" t="s">
+    <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A187" s="1" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="189" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A189" s="0" t="s">
+    <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A188" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="190" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A190" s="0" t="s">
+    <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A189" s="1" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="191" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A191" s="0" t="s">
+    <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A190" s="1" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="192" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A192" s="0" t="s">
+    <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A191" s="1" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="193" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A193" s="0" t="s">
+    <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A192" s="1" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="194" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A194" s="0" t="s">
+    <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A193" s="1" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="195" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A195" s="0" t="s">
+    <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A194" s="1" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="196" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A196" s="0" t="s">
+    <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A195" s="1" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="197" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A197" s="0" t="s">
+    <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A196" s="1" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="198" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A198" s="0" t="s">
+    <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A197" s="1" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="199" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A199" s="0" t="s">
+    <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A198" s="1" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="200" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A200" s="0" t="s">
+    <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A199" s="1" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="201" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A201" s="0" t="s">
+    <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A200" s="1" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="202" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A202" s="0" t="s">
+    <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A201" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="203" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A203" s="0" t="s">
+    <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A202" s="1" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="204" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A204" s="0" t="s">
+    <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A203" s="1" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="205" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A205" s="0" t="s">
+    <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A204" s="1" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="206" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A206" s="0" t="s">
+    <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A205" s="1" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="207" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A207" s="0" t="s">
+    <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A206" s="1" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="208" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A208" s="0" t="s">
+    <row r="207" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A207" s="1" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="209" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A209" s="0" t="s">
+    <row r="208" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A208" s="1" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="210" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A210" s="0" t="s">
+    <row r="209" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A209" s="1" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="211" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A211" s="0" t="s">
+    <row r="210" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A210" s="1" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="212" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A212" s="0" t="s">
+    <row r="211" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A211" s="1" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="213" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A213" s="0" t="s">
+    <row r="212" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A212" s="1" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="214" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A214" s="0" t="s">
+    <row r="213" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A213" s="1" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="215" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A215" s="0" t="s">
+    <row r="214" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A214" s="1" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="216" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A216" s="0" t="s">
+    <row r="215" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A215" s="1" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="217" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A217" s="0" t="s">
+    <row r="216" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A216" s="1" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="218" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A218" s="0" t="s">
+    <row r="217" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A217" s="1" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="219" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A219" s="0" t="s">
+    <row r="218" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A218" s="1" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="220" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A220" s="0" t="s">
+    <row r="219" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A219" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="221" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A221" s="0" t="s">
+    <row r="220" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A220" s="1" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="222" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A222" s="0" t="s">
+    <row r="221" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A221" s="1" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="223" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A223" s="0" t="s">
+    <row r="222" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A222" s="1" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="224" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A224" s="0" t="s">
+    <row r="223" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A223" s="1" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="225" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A225" s="0" t="s">
+    <row r="224" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A224" s="1" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="226" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A226" s="0" t="s">
+    <row r="225" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A225" s="1" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="227" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A227" s="0" t="s">
+    <row r="226" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A226" s="1" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="228" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A228" s="0" t="s">
+    <row r="227" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A227" s="1" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="229" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A229" s="0" t="s">
+    <row r="228" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A228" s="1" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="230" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A230" s="0" t="s">
+    <row r="229" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A229" s="1" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="231" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A231" s="0" t="s">
+    <row r="230" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A230" s="1" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="232" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A232" s="0" t="s">
+    <row r="231" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A231" s="1" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="233" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A233" s="0" t="s">
+    <row r="232" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A232" s="1" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="234" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A234" s="0" t="s">
+    <row r="233" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A233" s="1" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="235" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A235" s="0" t="s">
+    <row r="234" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A234" s="1" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="236" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A236" s="0" t="s">
+    <row r="235" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A235" s="1" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="237" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A237" s="0" t="s">
+    <row r="236" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A236" s="1" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="238" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A238" s="0" t="s">
+    <row r="237" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A237" s="1" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="239" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A239" s="0" t="s">
+    <row r="238" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A238" s="1" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="240" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A240" s="0" t="s">
+    <row r="239" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A239" s="1" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="241" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A241" s="0" t="s">
+    <row r="240" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A240" s="1" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="242" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A242" s="0" t="s">
+    <row r="241" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A241" s="1" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="243" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A243" s="0" t="s">
+    <row r="242" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A242" s="1" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="244" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A244" s="0" t="s">
+    <row r="243" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A243" s="1" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="245" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A245" s="0" t="s">
+    <row r="244" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A244" s="1" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="246" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A246" s="0" t="s">
+    <row r="245" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A245" s="1" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="247" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A247" s="0" t="s">
+    <row r="246" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A246" s="1" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="248" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A248" s="0" t="s">
+    <row r="247" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A247" s="1" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="249" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A249" s="0" t="s">
+    <row r="248" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A248" s="1" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="250" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A250" s="0" t="s">
+    <row r="249" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A249" s="1" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="251" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A251" s="0" t="s">
+    <row r="250" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A250" s="1" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="252" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A252" s="0" t="s">
+    <row r="251" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A251" s="1" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="253" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A253" s="0" t="s">
+    <row r="252" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A252" s="1" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="254" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A254" s="0" t="s">
+    <row r="253" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A253" s="1" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="255" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A255" s="0" t="s">
+    <row r="254" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A254" s="1" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="256" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A256" s="0" t="s">
+    <row r="255" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A255" s="1" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="257" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A257" s="0" t="s">
+    <row r="256" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A256" s="1" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="258" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A258" s="0" t="s">
+    <row r="257" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A257" s="1" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="259" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A259" s="0" t="s">
+    <row r="258" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A258" s="1" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="260" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A260" s="0" t="s">
+    <row r="259" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A259" s="1" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="261" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A261" s="0" t="s">
+    <row r="260" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A260" s="1" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="262" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A262" s="0" t="s">
+    <row r="261" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A261" s="1" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="263" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A263" s="0" t="s">
+    <row r="262" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A262" s="1" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="264" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A264" s="0" t="s">
+    <row r="263" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A263" s="1" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="265" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A265" s="0" t="s">
+    <row r="264" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A264" s="1" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="266" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A266" s="0" t="s">
+    <row r="265" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A265" s="1" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="267" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A267" s="0" t="s">
+    <row r="266" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A266" s="1" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="268" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A268" s="0" t="s">
+    <row r="267" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A267" s="1" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="269" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A269" s="0" t="s">
+    <row r="268" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A268" s="1" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="270" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A270" s="0" t="s">
+    <row r="269" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A269" s="1" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="271" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A271" s="0" t="s">
+    <row r="270" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A270" s="1" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="272" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A272" s="0" t="s">
+    <row r="271" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A271" s="1" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="273" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A273" s="0" t="s">
+    <row r="272" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A272" s="1" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="274" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A274" s="0" t="s">
+    <row r="273" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A273" s="1" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="275" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A275" s="0" t="s">
+    <row r="274" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A274" s="1" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="276" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A276" s="0" t="s">
+    <row r="275" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A275" s="1" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="277" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A277" s="0" t="s">
+    <row r="276" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A276" s="1" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="278" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A278" s="0" t="s">
+    <row r="277" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A277" s="1" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="279" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A279" s="0" t="s">
+    <row r="278" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A278" s="1" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="280" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A280" s="0" t="s">
+    <row r="279" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A279" s="1" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="281" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A281" s="0" t="s">
+    <row r="280" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A280" s="1" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="282" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A282" s="0" t="s">
+    <row r="281" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A281" s="1" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="283" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A283" s="0" t="s">
+    <row r="282" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A282" s="1" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="284" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A284" s="0" t="s">
+    <row r="283" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A283" s="1" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="285" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A285" s="0" t="s">
+    <row r="284" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A284" s="1" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="286" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A286" s="0" t="s">
+    <row r="285" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A285" s="1" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="287" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A287" s="0" t="s">
+    <row r="286" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A286" s="1" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="288" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A288" s="0" t="s">
+    <row r="287" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A287" s="1" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="289" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A289" s="0" t="s">
+    <row r="288" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A288" s="1" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="290" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A290" s="0" t="s">
+    <row r="289" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A289" s="1" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="291" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A291" s="0" t="s">
+    <row r="290" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A290" s="1" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="292" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A292" s="0" t="s">
+    <row r="291" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A291" s="1" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="293" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A293" s="0" t="s">
+    <row r="292" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A292" s="1" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="294" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A294" s="0" t="s">
+    <row r="293" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A293" s="1" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="295" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A295" s="0" t="s">
+    <row r="294" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A294" s="1" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="296" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A296" s="0" t="s">
+    <row r="295" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A295" s="1" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="297" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A297" s="0" t="s">
+    <row r="296" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A296" s="1" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="298" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A298" s="0" t="s">
+    <row r="297" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A297" s="1" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="299" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A299" s="0" t="s">
+    <row r="298" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A298" s="1" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="300" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A300" s="0" t="s">
+    <row r="299" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A299" s="1" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="301" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A301" s="0" t="s">
+    <row r="300" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A300" s="1" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="302" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A302" s="0" t="s">
+    <row r="301" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A301" s="1" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="303" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A303" s="0" t="s">
+    <row r="302" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A302" s="1" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="304" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A304" s="0" t="s">
+    <row r="303" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A303" s="1" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="305" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A305" s="0" t="s">
+    <row r="304" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A304" s="1" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="306" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A306" s="0" t="s">
+    <row r="305" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A305" s="1" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="307" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A307" s="0" t="s">
+    <row r="306" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A306" s="1" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="308" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A308" s="0" t="s">
+    <row r="307" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A307" s="1" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="309" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A309" s="0" t="s">
+    <row r="308" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A308" s="1" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="310" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A310" s="0" t="s">
+    <row r="309" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A309" s="1" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="311" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A311" s="0" t="s">
+    <row r="310" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A310" s="1" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="312" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A312" s="0" t="s">
+    <row r="311" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A311" s="1" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="313" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A313" s="0" t="s">
+    <row r="312" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A312" s="1" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="314" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A314" s="0" t="s">
+    <row r="313" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A313" s="1" t="s">
         <v>312</v>
       </c>
     </row>
+    <row r="314" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>